<commit_message>
Finishing the course offering backend Version
</commit_message>
<xml_diff>
--- a/lauCourseOffering_Backend/backend/sample.xlsx
+++ b/lauCourseOffering_Backend/backend/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1cf13879d774ffb/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1cf13879d774ffb/Desktop/Capstone/lauCourseOffering_Backend/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BBD04A8-870E-4E17-8DF4-C9B82DF40C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{5BBD04A8-870E-4E17-8DF4-C9B82DF40C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C510CB8F-C226-427D-B06C-881B9F9B791F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A35635DA-DD0C-41CA-A5ED-53B6087E0F70}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2687,10 +2686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2444A31F-324E-4384-B149-B47074EFC8F8}">
-  <dimension ref="A1:S628"/>
+  <dimension ref="A1:S630"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A614" workbookViewId="0">
+      <selection activeCell="E631" sqref="E631"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27775,6 +27774,78 @@
       <c r="R628" s="1"/>
       <c r="S628" s="1"/>
     </row>
+    <row r="629" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="D629">
+        <f>COUNTIF(D2:D628,"")</f>
+        <v>49</v>
+      </c>
+      <c r="E629">
+        <f t="shared" ref="E629:J629" si="0">COUNTIF(E2:E628,"")</f>
+        <v>103</v>
+      </c>
+      <c r="F629">
+        <f t="shared" si="0"/>
+        <v>326</v>
+      </c>
+      <c r="G629">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="H629">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="I629">
+        <f t="shared" si="0"/>
+        <v>347</v>
+      </c>
+      <c r="J629">
+        <f t="shared" si="0"/>
+        <v>329</v>
+      </c>
+      <c r="K629">
+        <f t="shared" ref="K629" si="1">COUNTIF(K2:K628,"")</f>
+        <v>605</v>
+      </c>
+      <c r="L629">
+        <f t="shared" ref="L629" si="2">COUNTIF(L2:L628,"")</f>
+        <v>509</v>
+      </c>
+      <c r="M629">
+        <f t="shared" ref="M629" si="3">COUNTIF(M2:M628,"")</f>
+        <v>530</v>
+      </c>
+      <c r="N629">
+        <f t="shared" ref="N629" si="4">COUNTIF(N2:N628,"")</f>
+        <v>429</v>
+      </c>
+      <c r="O629">
+        <f t="shared" ref="O629" si="5">COUNTIF(O2:O628,"")</f>
+        <v>553</v>
+      </c>
+      <c r="P629">
+        <f t="shared" ref="P629" si="6">COUNTIF(P2:P628,"")</f>
+        <v>595</v>
+      </c>
+      <c r="Q629">
+        <f t="shared" ref="Q629" si="7">COUNTIF(Q2:Q628,"")</f>
+        <v>572</v>
+      </c>
+      <c r="R629">
+        <f t="shared" ref="R629" si="8">COUNTIF(R2:R628,"")</f>
+        <v>385</v>
+      </c>
+      <c r="S629">
+        <f t="shared" ref="S629" si="9">COUNTIF(S2:S628,"")</f>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="630" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="E630">
+        <f>103-32</f>
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>